<commit_message>
le bon fichier de quotités de décharge
</commit_message>
<xml_diff>
--- a/quotite.xlsx
+++ b/quotite.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t xml:space="preserve">Syndicat</t>
   </si>
   <si>
-    <t xml:space="preserve">Quotité proposée</t>
+    <t xml:space="preserve">Quotité</t>
   </si>
   <si>
     <t xml:space="preserve">Ain (01)</t>
@@ -76,12 +76,18 @@
     <t xml:space="preserve">Cher (18)</t>
   </si>
   <si>
+    <t xml:space="preserve">Corrèze (19)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Côtes d'Armor (22)</t>
   </si>
   <si>
     <t xml:space="preserve">Deux-Sèvres (79)</t>
   </si>
   <si>
+    <t xml:space="preserve">Eure-et-Loire (28)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Essonne (91)</t>
   </si>
   <si>
@@ -130,7 +136,7 @@
     <t xml:space="preserve">Indre et Loire (37)</t>
   </si>
   <si>
-    <t xml:space="preserve">Limousin (19+23+87)</t>
+    <t xml:space="preserve">Limousin (23+87)</t>
   </si>
   <si>
     <t xml:space="preserve">Loir et Cher (41)</t>
@@ -142,7 +148,7 @@
     <t xml:space="preserve">Loire Atlantique (44)</t>
   </si>
   <si>
-    <t xml:space="preserve">Loiret (45+28)</t>
+    <t xml:space="preserve">Loiret (45)</t>
   </si>
   <si>
     <t xml:space="preserve">Lorraine (54+55+57+88)</t>
@@ -329,20 +335,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.14"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -365,7 +368,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0.557</v>
+        <v>0.588</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,7 +376,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.606</v>
+        <v>0.567</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,7 +384,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.479</v>
+        <v>0.466</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -389,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.931</v>
+        <v>0.948</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,7 +400,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>1.297</v>
+        <v>0.899</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,7 +408,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.503</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,7 +416,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.557</v>
+        <v>0.575</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,7 +424,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>1.139</v>
+        <v>1.087</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,7 +432,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.861</v>
+        <v>0.729</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,7 +440,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>1.208</v>
+        <v>1.156</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,7 +448,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.493</v>
+        <v>0.466</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -453,7 +456,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.976</v>
+        <v>0.765</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,7 +464,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.738</v>
+        <v>0.616</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -469,7 +472,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.596</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,7 +480,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.577</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,7 +488,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.738</v>
+        <v>0.478</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,7 +496,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>0.577</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,7 +504,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>1.071</v>
+        <v>0.575</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,7 +512,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>1.022</v>
+        <v>0.478</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +520,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>1.25</v>
+        <v>0.953</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,7 +528,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.785</v>
+        <v>1.018</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,7 +536,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>0.503</v>
+        <v>0.932</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,7 +544,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>1.996</v>
+        <v>0.749</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,7 +552,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>0.868</v>
+        <v>0.494</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,7 +560,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>1.103</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,7 +568,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>0.537</v>
+        <v>0.806</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +576,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>0.985</v>
+        <v>1.119</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,7 +584,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>0.684</v>
+        <v>0.506</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,7 +592,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>1.012</v>
+        <v>0.993</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,7 +600,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>1.227</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,7 +608,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>0.797</v>
+        <v>0.965</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,7 +616,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>0.464</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,7 +624,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>0.567</v>
+        <v>0.754</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,7 +632,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>0.885</v>
+        <v>0.445</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,7 +640,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>0.459</v>
+        <v>0.518</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,7 +648,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>0.665</v>
+        <v>0.676</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +656,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>0.816</v>
+        <v>0.449</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +664,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>0.902</v>
+        <v>0.697</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,7 +672,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>1.235</v>
+        <v>0.884</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,7 +680,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>0.518</v>
+        <v>0.757</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,7 +688,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>0.718</v>
+        <v>1.046</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,7 +696,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>1.031</v>
+        <v>0.506</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,7 +704,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>0.552</v>
+        <v>0.669</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,7 +712,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>0.621</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,7 +720,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>0.89</v>
+        <v>0.547</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,7 +728,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>1.036</v>
+        <v>0.604</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,7 +736,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>0.528</v>
+        <v>0.811</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -741,7 +744,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>0.611</v>
+        <v>1.075</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,7 +752,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>2.112</v>
+        <v>0.506</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,7 +760,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>0.811</v>
+        <v>0.575</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,7 +768,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>1.567</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,7 +776,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>0.78</v>
+        <v>0.783</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,7 +784,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>0.493</v>
+        <v>1.481</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -789,7 +792,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>1.296</v>
+        <v>0.741</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,7 +800,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>0.537</v>
+        <v>0.555</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,7 +808,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>0.87</v>
+        <v>1.392</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,7 +816,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>2.621</v>
+        <v>0.518</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,7 +824,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>0.591</v>
+        <v>0.787</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -829,7 +832,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>0.64</v>
+        <v>2.221</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,7 +840,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>0.758</v>
+        <v>0.555</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,7 +848,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>1.164</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,7 +856,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>0.714</v>
+        <v>0.774</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -861,7 +864,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>0.67</v>
+        <v>1.051</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,7 +872,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>0.826</v>
+        <v>0.685</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,7 +880,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>0.577</v>
+        <v>0.547</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,7 +888,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>0.621</v>
+        <v>0.754</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,7 +896,7 @@
         <v>69</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>0.611</v>
+        <v>0.583</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,13 +904,29 @@
         <v>70</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>57.997</v>
+        <v>0.559</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="1" t="n">
+        <v>0.575</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="1" t="n">
+        <v>54.505</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>